<commit_message>
Dana einda: VSC da POWERBI
</commit_message>
<xml_diff>
--- a/data/processed/accidentes_victimas_comun_auton.xlsx
+++ b/data/processed/accidentes_victimas_comun_auton.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Downloads\proyecto_accidentes\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C191B45-9454-48AC-AE5A-DC7D569D0C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9CEFCA-4BE1-4A39-9398-9F8C1BE5C8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{320FB97E-1D06-468B-9846-EBCB93BA65FD}"/>
   </bookViews>
@@ -33,10 +33,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>ACCIDENTES CON
-VÍCTIMAS</t>
-  </si>
-  <si>
     <t>ACCIDENTES
 MORTALES</t>
   </si>
@@ -104,6 +100,9 @@
   </si>
   <si>
     <t>Ceuta y Melilla</t>
+  </si>
+  <si>
+    <t>ACCIDENTES CON VÍCTIMAS</t>
   </si>
 </sst>
 </file>
@@ -551,7 +550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E9B4EA-EAC8-413B-A64B-CA69898EF0EC}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
@@ -567,24 +568,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>17367</v>
@@ -604,7 +605,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>2185</v>
@@ -624,7 +625,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>1842</v>
@@ -644,7 +645,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>2871</v>
@@ -664,7 +665,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>4270</v>
@@ -684,7 +685,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>1180</v>
@@ -704,7 +705,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>2928</v>
@@ -724,7 +725,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>3946</v>
@@ -744,7 +745,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>23590</v>
@@ -764,7 +765,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>1542</v>
@@ -784,7 +785,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
         <v>4605</v>
@@ -804,7 +805,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
         <v>14680</v>
@@ -824,7 +825,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>3464</v>
@@ -844,7 +845,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
         <v>704</v>
@@ -864,7 +865,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>686</v>
@@ -884,7 +885,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>10220</v>
@@ -904,7 +905,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>4467</v>
@@ -924,7 +925,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
         <v>759</v>

</xml_diff>